<commit_message>
Created react class based components
</commit_message>
<xml_diff>
--- a/project-status-report.xlsx
+++ b/project-status-report.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Project Status Report</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Project Name</t>
   </si>
@@ -38,12 +35,6 @@
     <t>Project Manager</t>
   </si>
   <si>
-    <t>Status Date</t>
-  </si>
-  <si>
-    <t>Project Ket Parameters</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
@@ -56,35 +47,101 @@
     <t>Budget</t>
   </si>
   <si>
-    <t>Issues</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Project Schedule</t>
-  </si>
-  <si>
-    <t>Project Risks and Issues (Top 5)</t>
-  </si>
-  <si>
-    <t>Risk/Issue</t>
-  </si>
-  <si>
-    <t>Risk/Issue Desciption</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Week Ending</t>
+  </si>
+  <si>
+    <t>Project Phase</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Finish Date</t>
+  </si>
+  <si>
+    <t>Revised Finish Date</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
+  </si>
+  <si>
+    <t>Initial Value</t>
+  </si>
+  <si>
+    <t>Revised Project Plan</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>Project Key Parameters</t>
+  </si>
+  <si>
+    <t>Week N-2</t>
+  </si>
+  <si>
+    <t>Week N-1</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Risk &amp; Issues</t>
+  </si>
+  <si>
+    <t>Resourcing</t>
+  </si>
+  <si>
+    <t>MILESTONES</t>
+  </si>
+  <si>
+    <t>Milestone</t>
+  </si>
+  <si>
+    <t>Baseline Date</t>
+  </si>
+  <si>
+    <t>Latest Forecast</t>
+  </si>
+  <si>
+    <t>Actual Date</t>
+  </si>
+  <si>
+    <t>PROGRESS SUMMARY</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Target Date</t>
+  </si>
+  <si>
+    <t>KEY RISKS, ISSUES &amp; DEPENDENCIES</t>
+  </si>
+  <si>
+    <t>PROJECT STATUS REPORT</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +149,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -109,12 +193,220 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,97 +687,451 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="25"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="29"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
     </row>
   </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F26"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>